<commit_message>
Update BOM for low profile el. capacitors.
</commit_message>
<xml_diff>
--- a/Modules/KickAid/KickAid_BOM.xlsx
+++ b/Modules/KickAid/KickAid_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\KickAid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA46282-2DE1-4FB0-BF63-F34CB52A9B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A916A342-D823-4379-8B5F-366140462A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,13 +359,7 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>https://www.thonk.co.uk/shop/eurorack-diy-essentials/</t>
-  </si>
-  <si>
     <t>C3, C4, C5</t>
-  </si>
-  <si>
-    <t>* Needs to be a low profile capacitor.</t>
   </si>
   <si>
     <t>C6</t>
@@ -752,8 +746,17 @@
     <t>C-P5mm</t>
   </si>
   <si>
+    <t>E-P2.5mm 6.3x11.5mm</t>
+  </si>
+  <si>
+    <t>Electrolytic Capacitor THT</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor THT</t>
+  </si>
+  <si>
     <r>
-      <t>E-P2.5mm 5x5mm</t>
+      <t>E-P2.5mm 5x7mm</t>
     </r>
     <r>
       <rPr>
@@ -768,13 +771,10 @@
     </r>
   </si>
   <si>
-    <t>E-P2.5mm 6.3x11.5mm</t>
-  </si>
-  <si>
-    <t>Electrolytic Capacitor THT</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor THT</t>
+    <t>https://www.tme.eu/hr/en/details/ecea1vka100i/tht-electrolytic-capacitors/panasonic/</t>
+  </si>
+  <si>
+    <t>* Needs to be a low profile capacitor, maximum of 7mm in height.</t>
   </si>
 </sst>
 </file>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,10 +1730,10 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1750,7 +1750,7 @@
         <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>70</v>
@@ -1770,7 +1770,7 @@
         <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
         <v>82</v>
@@ -1790,10 +1790,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1810,7 +1810,7 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
         <v>84</v>
@@ -1830,10 +1830,10 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -1850,7 +1850,7 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
         <v>95</v>
@@ -1870,7 +1870,7 @@
         <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
         <v>86</v>
@@ -1890,7 +1890,7 @@
         <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D10" t="s">
         <v>96</v>
@@ -1910,7 +1910,7 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>87</v>
@@ -1930,10 +1930,10 @@
         <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
@@ -1950,10 +1950,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
@@ -1970,7 +1970,7 @@
         <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D14" t="s">
         <v>90</v>
@@ -1996,7 +1996,7 @@
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>97</v>
@@ -2016,10 +2016,10 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>75</v>
@@ -2042,7 +2042,7 @@
         <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>72</v>
@@ -2059,13 +2059,13 @@
         <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>77</v>
@@ -2076,19 +2076,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" t="s">
         <v>104</v>
       </c>
-      <c r="C19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D19" t="s">
-        <v>106</v>
-      </c>
       <c r="E19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2099,13 +2099,13 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -2119,16 +2119,16 @@
         <v>99</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2139,13 +2139,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>30</v>
@@ -2182,7 +2182,7 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
@@ -2196,19 +2196,19 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
         <v>107</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F25" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2219,10 +2219,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E26" t="s">
         <v>23</v>
@@ -2242,7 +2242,7 @@
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E27" t="s">
         <v>23</v>
@@ -2262,7 +2262,7 @@
         <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
@@ -2276,19 +2276,19 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2296,19 +2296,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
+      <c r="F30" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2316,19 +2316,19 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -2336,19 +2336,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" t="s">
         <v>126</v>
       </c>
-      <c r="C32" t="s">
+      <c r="F32" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2356,13 +2356,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -2376,13 +2376,13 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" t="s">
         <v>144</v>
       </c>
-      <c r="C34" t="s">
-        <v>146</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
@@ -2396,19 +2396,19 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,19 +2416,19 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2436,19 +2436,19 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,19 +2456,19 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C38" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E38" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2476,19 +2476,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" t="s">
         <v>133</v>
       </c>
-      <c r="C39" t="s">
+      <c r="F39" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E39" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2496,19 +2496,19 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" t="s">
         <v>149</v>
       </c>
-      <c r="C40" t="s">
+      <c r="F40" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2519,10 +2519,10 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
         <v>80</v>
@@ -2536,13 +2536,13 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
         <v>21</v>
@@ -2562,7 +2562,7 @@
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -2576,13 +2576,13 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -2602,7 +2602,7 @@
         <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -2616,13 +2616,13 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -2744,13 +2744,13 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E55" t="s">
         <v>49</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2778,13 +2778,13 @@
         <v>41</v>
       </c>
       <c r="C57" t="s">
+        <v>162</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="E57" t="s">
-        <v>165</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2797,17 +2797,17 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2868,8 +2868,9 @@
     <hyperlink ref="F40" r:id="rId54" xr:uid="{932A7A9F-0EC3-41B4-8980-42A6D5FC0033}"/>
     <hyperlink ref="F57" r:id="rId55" xr:uid="{7A52BB5F-2156-4696-A05E-A65CF92F76E9}"/>
     <hyperlink ref="F55" r:id="rId56" xr:uid="{2CBD1E2B-EA04-41D5-947D-738E19704CE1}"/>
+    <hyperlink ref="F21" r:id="rId57" xr:uid="{D7D22B2B-3A31-4EBC-A56A-9A899E1E05E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document a fix for a buzzing issue on KickAid.
</commit_message>
<xml_diff>
--- a/Modules/KickAid/KickAid_BOM.xlsx
+++ b/Modules/KickAid/KickAid_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\KickAid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A916A342-D823-4379-8B5F-366140462A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E13F20-33F6-47F4-B62F-C68FD4F6DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="185">
   <si>
     <t>Qty</t>
   </si>
@@ -518,9 +518,6 @@
     <t>SW_SRC</t>
   </si>
   <si>
-    <t>J_EXT, J_TRIG, J_GATE, J_ENV, J_IN, J_SND, J_RET, J_OUT</t>
-  </si>
-  <si>
     <t>1x6</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
   </si>
   <si>
     <t>** Use the included extra nut as a washer between the switch and the panel.</t>
-  </si>
-  <si>
-    <t>*** For P_IN, P_EQ_K and P_EQ_F, do not use the included washer. Tighten very gently so the PCB doesn't get scratched. Install P_MIX normally.</t>
   </si>
   <si>
     <t>Thonk Trimmer Topper</t>
@@ -611,33 +605,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>D7-D12</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Alpha 9mm Nut</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>**</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
     </r>
   </si>
   <si>
@@ -776,12 +743,73 @@
   <si>
     <t>* Needs to be a low profile capacitor, maximum of 7mm in height.</t>
   </si>
+  <si>
+    <r>
+      <t>Alpha 9mm Nut</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>***</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J_EXT, J_TRIG, J_GATE, J_ENV, J_IN</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>***</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, J_SND, J_RET, J_OUT</t>
+    </r>
+  </si>
+  <si>
+    <t>**** For P_IN, P_EQ_K and P_EQ_F, do not use the included washer. Tighten very gently so the PCB doesn't get scratched. Install P_MIX normally.</t>
+  </si>
+  <si>
+    <t>*** IMPORTANT: An issue has been identified on KickAid, which causes a buzzing sound when GAIN is set to high and there is nothing plugged into the IN jack. Please solder the 2 joints together like shown on the image below to fix this. This will be fixed on board level on next revision.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -979,6 +1007,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1396,6 +1432,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2159000</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7594C797-71DB-A4B9-6C63-5D669D7368E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="12382500"/>
+          <a:ext cx="5778500" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1685,10 +1776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,7 +1787,7 @@
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" customWidth="1"/>
     <col min="5" max="5" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
@@ -1730,10 +1821,10 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1750,7 +1841,7 @@
         <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>70</v>
@@ -1770,7 +1861,7 @@
         <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
         <v>82</v>
@@ -1790,10 +1881,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1810,7 +1901,7 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
         <v>84</v>
@@ -1830,10 +1921,10 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -1850,7 +1941,7 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
         <v>95</v>
@@ -1870,7 +1961,7 @@
         <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
         <v>86</v>
@@ -1890,7 +1981,7 @@
         <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D10" t="s">
         <v>96</v>
@@ -1910,7 +2001,7 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>87</v>
@@ -1930,7 +2021,7 @@
         <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
         <v>110</v>
@@ -1950,10 +2041,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
@@ -1970,7 +2061,7 @@
         <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
         <v>90</v>
@@ -1996,7 +2087,7 @@
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>97</v>
@@ -2016,10 +2107,10 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>75</v>
@@ -2042,7 +2133,7 @@
         <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>72</v>
@@ -2059,13 +2150,13 @@
         <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
         <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>77</v>
@@ -2079,13 +2170,13 @@
         <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
         <v>104</v>
       </c>
       <c r="E19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>103</v>
@@ -2099,13 +2190,13 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" t="s">
         <v>177</v>
-      </c>
-      <c r="D20" t="s">
-        <v>170</v>
-      </c>
-      <c r="E20" t="s">
-        <v>180</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -2119,16 +2210,16 @@
         <v>99</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E21" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2139,13 +2230,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>30</v>
@@ -2182,7 +2273,7 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
@@ -2519,7 +2610,7 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>152</v>
@@ -2536,13 +2627,13 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="E42" t="s">
         <v>21</v>
@@ -2562,7 +2653,7 @@
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -2576,13 +2667,13 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -2602,7 +2693,7 @@
         <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -2616,13 +2707,13 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -2744,13 +2835,13 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="E55" t="s">
         <v>49</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2778,13 +2869,13 @@
         <v>41</v>
       </c>
       <c r="C57" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="E57" t="s">
-        <v>163</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2797,17 +2888,22 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>161</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2872,5 +2968,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
+  <drawing r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Better description for the fix, and better picture.
</commit_message>
<xml_diff>
--- a/Modules/KickAid/KickAid_BOM.xlsx
+++ b/Modules/KickAid/KickAid_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\KickAid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E13F20-33F6-47F4-B62F-C68FD4F6DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66D9EFF-081E-46BA-B531-A0969972B4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,7 +802,7 @@
     <t>**** For P_IN, P_EQ_K and P_EQ_F, do not use the included washer. Tighten very gently so the PCB doesn't get scratched. Install P_MIX normally.</t>
   </si>
   <si>
-    <t>*** IMPORTANT: An issue has been identified on KickAid, which causes a buzzing sound when GAIN is set to high and there is nothing plugged into the IN jack. Please solder the 2 joints together like shown on the image below to fix this. This will be fixed on board level on next revision.</t>
+    <t>*** IMPORTANT: If you have v1.1 board, please solder the 2 joints together like shown on the image below.Otherwise, a buzzing sound could be heard when GAIN is set to high and there is nothing plugged into the IN jack.</t>
   </si>
 </sst>
 </file>
@@ -1439,22 +1439,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2159000</xdr:colOff>
+      <xdr:colOff>357822</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7594C797-71DB-A4B9-6C63-5D669D7368E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44CE7730-1554-4F72-81DC-038292537D7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1470,14 +1470,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="361950" y="12382500"/>
-          <a:ext cx="5778500" cy="4333875"/>
+          <a:off x="381000" y="12392025"/>
+          <a:ext cx="3958272" cy="4333875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1778,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61:B64"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clarify that it is v1.0 Front Board, not v1.1.
</commit_message>
<xml_diff>
--- a/Modules/KickAid/KickAid_BOM.xlsx
+++ b/Modules/KickAid/KickAid_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\KickAid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66D9EFF-081E-46BA-B531-A0969972B4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270CF69-C4EB-4D15-9EAF-4E9C0A2FAE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,7 +802,7 @@
     <t>**** For P_IN, P_EQ_K and P_EQ_F, do not use the included washer. Tighten very gently so the PCB doesn't get scratched. Install P_MIX normally.</t>
   </si>
   <si>
-    <t>*** IMPORTANT: If you have v1.1 board, please solder the 2 joints together like shown on the image below.Otherwise, a buzzing sound could be heard when GAIN is set to high and there is nothing plugged into the IN jack.</t>
+    <t>*** IMPORTANT: If you have v1.0 Front Board, please solder the 2 joints together like shown on the image below.Otherwise, a buzzing sound could be heard when GAIN is set to high and there is nothing plugged into the IN jack.</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1447,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>357822</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1476,7 +1476,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="381000" y="12392025"/>
-          <a:ext cx="3958272" cy="4333875"/>
+          <a:ext cx="3958272" cy="4333874"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1777,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update KickAid BOM and Schematic.
</commit_message>
<xml_diff>
--- a/Modules/KickAid/KickAid_BOM.xlsx
+++ b/Modules/KickAid/KickAid_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\KickAid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270CF69-C4EB-4D15-9EAF-4E9C0A2FAE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CEA4F8-B7A6-4A39-BA34-256E5E7EFE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KickAid" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="184">
   <si>
     <t>Qty</t>
   </si>
@@ -293,9 +293,6 @@
     <t>15k</t>
   </si>
   <si>
-    <t>R13, R14, R15, R16</t>
-  </si>
-  <si>
     <t>R17</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
   </si>
   <si>
     <t>160k</t>
-  </si>
-  <si>
-    <t>R27, R28</t>
   </si>
   <si>
     <r>
@@ -362,18 +356,6 @@
     <t>C3, C4, C5</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>100pF</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/cm-100/mlcc-tht-capacitors/sr-passives/</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
     <t>BCM847BS</t>
   </si>
   <si>
@@ -558,22 +540,6 @@
   </si>
   <si>
     <t>https://www.thonk.co.uk/shop/tall-trimmer-toppers/</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">R10, R11, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R12</t>
-    </r>
   </si>
   <si>
     <r>
@@ -800,6 +766,37 @@
   </si>
   <si>
     <t>**** For P_IN, P_EQ_K and P_EQ_F, do not use the included washer. Tighten very gently so the PCB doesn't get scratched. Install P_MIX normally.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R11, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R12</t>
+    </r>
+  </si>
+  <si>
+    <t>C6, C22</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>120k</t>
+  </si>
+  <si>
+    <t>R10, R13, R14, R15, R16</t>
   </si>
   <si>
     <t>*** IMPORTANT: If you have v1.0 Front Board, please solder the 2 joints together like shown on the image below.Otherwise, a buzzing sound could be heard when GAIN is set to high and there is nothing plugged into the IN jack.</t>
@@ -1777,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,10 +1817,10 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1840,7 +1837,7 @@
         <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>70</v>
@@ -1860,7 +1857,7 @@
         <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
         <v>82</v>
@@ -1880,10 +1877,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1900,7 +1897,7 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
         <v>84</v>
@@ -1914,16 +1911,16 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -1937,33 +1934,33 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -1977,19 +1974,19 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2000,10 +1997,10 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -2017,13 +2014,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
@@ -2040,10 +2037,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
@@ -2054,16 +2051,16 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -2077,42 +2074,39 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>74</v>
+        <v>166</v>
+      </c>
+      <c r="D15" t="s">
+        <v>179</v>
       </c>
       <c r="E15" t="s">
-        <v>170</v>
+        <v>16</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" t="s">
-        <v>164</v>
+      <c r="D16" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>73</v>
@@ -2120,22 +2114,22 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="E17" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>73</v>
@@ -2143,42 +2137,45 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2189,13 +2186,13 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D20" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E20" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -2206,19 +2203,19 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2229,13 +2226,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>30</v>
@@ -2272,7 +2269,7 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
@@ -2286,19 +2283,19 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2309,10 +2306,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E26" t="s">
         <v>23</v>
@@ -2332,7 +2329,7 @@
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
         <v>23</v>
@@ -2352,7 +2349,7 @@
         <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
@@ -2366,19 +2363,19 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2386,19 +2383,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2406,19 +2403,19 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E31" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -2426,19 +2423,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E32" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2446,13 +2443,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -2466,13 +2463,13 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
@@ -2486,19 +2483,19 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2506,19 +2503,19 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="E36" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2526,19 +2523,19 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2546,19 +2543,19 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,19 +2563,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E39" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,19 +2583,19 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2609,10 +2606,10 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
         <v>80</v>
@@ -2626,13 +2623,13 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E42" t="s">
         <v>21</v>
@@ -2652,7 +2649,7 @@
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -2666,13 +2663,13 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -2692,7 +2689,7 @@
         <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -2706,13 +2703,13 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -2834,13 +2831,13 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E55" t="s">
         <v>49</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2868,13 +2865,13 @@
         <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E57" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2887,22 +2884,22 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2923,11 +2920,11 @@
     <hyperlink ref="F45" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="F43" r:id="rId15" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
     <hyperlink ref="F47" r:id="rId16" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
-    <hyperlink ref="P16" r:id="rId17" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
-    <hyperlink ref="P17" r:id="rId18" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
-    <hyperlink ref="F17" r:id="rId19" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
-    <hyperlink ref="F16" r:id="rId20" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
-    <hyperlink ref="F18" r:id="rId21" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
+    <hyperlink ref="P17" r:id="rId17" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
+    <hyperlink ref="P18" r:id="rId18" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
+    <hyperlink ref="F18" r:id="rId19" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
+    <hyperlink ref="F17" r:id="rId20" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
+    <hyperlink ref="F19" r:id="rId21" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
     <hyperlink ref="F44" r:id="rId22" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
     <hyperlink ref="F46" r:id="rId23" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
     <hyperlink ref="F41" r:id="rId24" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
@@ -2941,29 +2938,29 @@
     <hyperlink ref="F6" r:id="rId32" xr:uid="{58A8E3CE-CD3F-43A3-B946-EE7AAC959BB8}"/>
     <hyperlink ref="F9" r:id="rId33" xr:uid="{B4611C36-E3CD-48A1-B558-378FFEE572B7}"/>
     <hyperlink ref="F12" r:id="rId34" xr:uid="{40377A08-FCE6-4F89-9187-96A00B93A312}"/>
-    <hyperlink ref="F14" r:id="rId35" xr:uid="{5A1179F6-3A84-498D-87AF-DBF1D5EAF071}"/>
+    <hyperlink ref="F15" r:id="rId35" xr:uid="{5A1179F6-3A84-498D-87AF-DBF1D5EAF071}"/>
     <hyperlink ref="F8" r:id="rId36" xr:uid="{F2E3BA95-EDCE-4952-9E03-A8804711C4CB}"/>
     <hyperlink ref="F10" r:id="rId37" xr:uid="{4C536C75-1E7B-4E8E-AC70-3B143F26311E}"/>
-    <hyperlink ref="P15" r:id="rId38" xr:uid="{9DE94678-EFDC-4596-B004-CE73B42552E7}"/>
-    <hyperlink ref="F15" r:id="rId39" xr:uid="{22025D74-97DB-4D2B-BB71-13FAD64FC821}"/>
-    <hyperlink ref="F19" r:id="rId40" xr:uid="{0C6BC1DA-66E4-4473-9F52-78D8E7579C0F}"/>
-    <hyperlink ref="F25" r:id="rId41" xr:uid="{0DF77104-940B-4656-902E-D3B4A729F975}"/>
-    <hyperlink ref="F29" r:id="rId42" xr:uid="{0234E1EC-3124-4C89-975E-D13FE095B07F}"/>
-    <hyperlink ref="F30" r:id="rId43" xr:uid="{DB5928A3-0C2C-41C8-94E2-173BFEB2B0BB}"/>
-    <hyperlink ref="F31" r:id="rId44" xr:uid="{24D2838B-698C-49F3-A89F-82FDF5909F9B}"/>
-    <hyperlink ref="F32" r:id="rId45" xr:uid="{5354C7EC-6A56-490A-97A1-06170A361210}"/>
-    <hyperlink ref="F26" r:id="rId46" xr:uid="{DA65564B-FC06-44AA-BE9E-CDEC85344EA4}"/>
-    <hyperlink ref="F35" r:id="rId47" xr:uid="{9B529563-7FF1-4CBB-B28F-CF26D80CBBD0}"/>
-    <hyperlink ref="F36" r:id="rId48" xr:uid="{19B2C35A-2AC5-48E0-ADAA-8A862A2BE8D1}"/>
-    <hyperlink ref="F38" r:id="rId49" xr:uid="{95AFB553-4A2D-4412-8ADD-9C777E0114C2}"/>
-    <hyperlink ref="F39" r:id="rId50" xr:uid="{B4A17999-A824-419D-96B6-45991272181C}"/>
-    <hyperlink ref="F37" r:id="rId51" xr:uid="{748FCFF4-A3F0-42DC-A53F-B6C8D0F870A5}"/>
-    <hyperlink ref="F34" r:id="rId52" xr:uid="{8CE5E525-65D3-417D-A66F-FDAA297CA9FB}"/>
-    <hyperlink ref="F33" r:id="rId53" xr:uid="{DF66115C-265B-4566-AA35-F0AD032F438C}"/>
-    <hyperlink ref="F40" r:id="rId54" xr:uid="{932A7A9F-0EC3-41B4-8980-42A6D5FC0033}"/>
-    <hyperlink ref="F57" r:id="rId55" xr:uid="{7A52BB5F-2156-4696-A05E-A65CF92F76E9}"/>
-    <hyperlink ref="F55" r:id="rId56" xr:uid="{2CBD1E2B-EA04-41D5-947D-738E19704CE1}"/>
-    <hyperlink ref="F21" r:id="rId57" xr:uid="{D7D22B2B-3A31-4EBC-A56A-9A899E1E05E5}"/>
+    <hyperlink ref="P16" r:id="rId38" xr:uid="{9DE94678-EFDC-4596-B004-CE73B42552E7}"/>
+    <hyperlink ref="F16" r:id="rId39" xr:uid="{22025D74-97DB-4D2B-BB71-13FAD64FC821}"/>
+    <hyperlink ref="F25" r:id="rId40" xr:uid="{0DF77104-940B-4656-902E-D3B4A729F975}"/>
+    <hyperlink ref="F29" r:id="rId41" xr:uid="{0234E1EC-3124-4C89-975E-D13FE095B07F}"/>
+    <hyperlink ref="F30" r:id="rId42" xr:uid="{DB5928A3-0C2C-41C8-94E2-173BFEB2B0BB}"/>
+    <hyperlink ref="F31" r:id="rId43" xr:uid="{24D2838B-698C-49F3-A89F-82FDF5909F9B}"/>
+    <hyperlink ref="F32" r:id="rId44" xr:uid="{5354C7EC-6A56-490A-97A1-06170A361210}"/>
+    <hyperlink ref="F26" r:id="rId45" xr:uid="{DA65564B-FC06-44AA-BE9E-CDEC85344EA4}"/>
+    <hyperlink ref="F35" r:id="rId46" xr:uid="{9B529563-7FF1-4CBB-B28F-CF26D80CBBD0}"/>
+    <hyperlink ref="F36" r:id="rId47" xr:uid="{19B2C35A-2AC5-48E0-ADAA-8A862A2BE8D1}"/>
+    <hyperlink ref="F38" r:id="rId48" xr:uid="{95AFB553-4A2D-4412-8ADD-9C777E0114C2}"/>
+    <hyperlink ref="F39" r:id="rId49" xr:uid="{B4A17999-A824-419D-96B6-45991272181C}"/>
+    <hyperlink ref="F37" r:id="rId50" xr:uid="{748FCFF4-A3F0-42DC-A53F-B6C8D0F870A5}"/>
+    <hyperlink ref="F34" r:id="rId51" xr:uid="{8CE5E525-65D3-417D-A66F-FDAA297CA9FB}"/>
+    <hyperlink ref="F33" r:id="rId52" xr:uid="{DF66115C-265B-4566-AA35-F0AD032F438C}"/>
+    <hyperlink ref="F40" r:id="rId53" xr:uid="{932A7A9F-0EC3-41B4-8980-42A6D5FC0033}"/>
+    <hyperlink ref="F57" r:id="rId54" xr:uid="{7A52BB5F-2156-4696-A05E-A65CF92F76E9}"/>
+    <hyperlink ref="F55" r:id="rId55" xr:uid="{2CBD1E2B-EA04-41D5-947D-738E19704CE1}"/>
+    <hyperlink ref="F21" r:id="rId56" xr:uid="{D7D22B2B-3A31-4EBC-A56A-9A899E1E05E5}"/>
+    <hyperlink ref="F14" r:id="rId57" xr:uid="{67316A66-E885-4019-9B97-023E307D9CB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>

</xml_diff>

<commit_message>
Change a resistor on KickAid for better AC coupling.
</commit_message>
<xml_diff>
--- a/Modules/KickAid/KickAid_BOM.xlsx
+++ b/Modules/KickAid/KickAid_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\KickAid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4337C7E0-8BD0-44FD-AE59-26AFCC301E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B5E91B-B34F-48F1-B26B-C29CE333B191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="206">
   <si>
     <t>Qty</t>
   </si>
@@ -679,6 +679,669 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">RN2, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RN3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C7-C18, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, C20, C21, C23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">D3-D6, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_EQ_K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_EQ_F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_MIX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_THRS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_DUCK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LD_K</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LD_F</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LD_G</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LD_E</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_EXT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_TRIG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_GATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_ENV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>***</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_SND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_RET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_OUT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> J_B3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> J_B6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> J_B7</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p041/73P0029/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p043/73P0031/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p044/73P0032/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p046/73P0034/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p048/73P0036/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p050/73P0038/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p052/73P0040/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p053/73P0041/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p054/73P0042/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/icvt-14p/standard-dip-sockets/connfly/ds1009-14at1nx-0a2/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/icvt-8p/standard-dip-sockets/connfly/ds1009-08at1nx/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/zl262-6sg/pin-headers/connfly/ds1023-1-6s21/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/zl262-4sg/pin-headers/connfly/ds1023-1-4s21/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c1502fct00/14E605/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c1203fct00/14E715/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c1603fct00/14E730/</t>
+  </si>
+  <si>
+    <t>240k</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">R24, R25, </t>
     </r>
     <r>
@@ -700,665 +1363,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, R33, R34</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">RN2, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RN3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">C7-C18, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, C20, C21, C23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">D3-D6, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D12</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_EQ_K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_EQ_F</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_MIX</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_THRS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_DUCK</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LD_K</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LD_F</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LD_G</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LD_E</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_EXT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_TRIG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_GATE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_ENV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_IN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>***</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_SND</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_RET</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_OUT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_B1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> J_B3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_B5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_B2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_B4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> J_B6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> J_B7</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p041/73P0029/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p043/73P0031/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p044/73P0032/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p046/73P0034/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p048/73P0036/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p050/73P0038/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p052/73P0040/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p053/73P0041/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p054/73P0042/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/icvt-14p/standard-dip-sockets/connfly/ds1009-14at1nx-0a2/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/icvt-8p/standard-dip-sockets/connfly/ds1009-08at1nx/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/zl262-6sg/pin-headers/connfly/ds1023-1-6s21/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/zl262-4sg/pin-headers/connfly/ds1023-1-4s21/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c1502fct00/14E605/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c1203fct00/14E715/</t>
-  </si>
-  <si>
-    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c1603fct00/14E730/</t>
+      <t>, R33</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/vishay/wirewound-resistors/mba02040c2403fct00/14E750/</t>
   </si>
 </sst>
 </file>
@@ -2006,13 +2015,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>357822</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2341,10 +2350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,7 +2412,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>27</v>
@@ -2426,7 +2435,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>27</v>
@@ -2449,7 +2458,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>27</v>
@@ -2472,7 +2481,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>27</v>
@@ -2495,7 +2504,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>27</v>
@@ -2518,7 +2527,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>27</v>
@@ -2544,7 +2553,7 @@
         <v>152</v>
       </c>
       <c r="J9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2567,7 +2576,7 @@
         <v>27</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2590,7 +2599,7 @@
         <v>153</v>
       </c>
       <c r="J11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2610,7 +2619,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>27</v>
@@ -2633,7 +2642,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>27</v>
@@ -2641,7 +2650,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -2650,13 +2659,13 @@
         <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>27</v>
@@ -2682,7 +2691,7 @@
         <v>27</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2705,7 +2714,7 @@
         <v>27</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2713,36 +2722,36 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>65</v>
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>203</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>154</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
-        <v>176</v>
+      <c r="D18" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E18" t="s">
         <v>132</v>
@@ -2751,21 +2760,21 @@
         <v>64</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
         <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="E19" t="s">
         <v>132</v>
@@ -2774,99 +2783,99 @@
         <v>64</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J20" t="s">
-        <v>197</v>
+        <v>64</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
         <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
         <v>139</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>140</v>
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>137</v>
+        <v>83</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>177</v>
       </c>
       <c r="E23" t="s">
         <v>138</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2874,68 +2883,68 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2943,36 +2952,36 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>96</v>
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J27" t="s">
         <v>196</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="E28" t="s">
         <v>23</v>
@@ -2986,48 +2995,48 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="J29" t="s">
-        <v>197</v>
+        <v>194</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3035,22 +3044,22 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>96</v>
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3058,22 +3067,22 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3081,22 +3090,22 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3104,36 +3113,36 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>118</v>
+        <v>100</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="J34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
         <v>117</v>
       </c>
-      <c r="D35" t="s">
-        <v>180</v>
+      <c r="D35" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="E35" t="s">
         <v>58</v>
@@ -3142,30 +3151,30 @@
         <v>29</v>
       </c>
       <c r="J35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>109</v>
+        <v>117</v>
+      </c>
+      <c r="D36" t="s">
+        <v>179</v>
       </c>
       <c r="E36" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="J36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3173,13 +3182,13 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
         <v>106</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
         <v>107</v>
@@ -3187,19 +3196,22 @@
       <c r="F37" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="J37" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
         <v>106</v>
       </c>
-      <c r="D38" t="s">
-        <v>181</v>
+      <c r="D38" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="E38" t="s">
         <v>107</v>
@@ -3210,16 +3222,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
         <v>106</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>114</v>
+      <c r="D39" t="s">
+        <v>180</v>
       </c>
       <c r="E39" t="s">
         <v>107</v>
@@ -3233,13 +3245,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
         <v>106</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" t="s">
         <v>107</v>
@@ -3250,108 +3262,105 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>182</v>
+        <v>106</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="J41" t="s">
-        <v>197</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="E42" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="J42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" t="s">
-        <v>183</v>
+        <v>126</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="E43" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="J43" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>170</v>
+        <v>31</v>
       </c>
       <c r="J44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
         <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -3360,44 +3369,44 @@
         <v>170</v>
       </c>
       <c r="J45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>184</v>
+        <v>125</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>59</v>
+        <v>170</v>
+      </c>
+      <c r="J46" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
       </c>
       <c r="D47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
@@ -3411,45 +3420,48 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="J48" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>3</v>
-      </c>
-      <c r="B50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J50" t="s">
-        <v>197</v>
+      <c r="J49" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3457,19 +3469,19 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E51" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3477,47 +3489,47 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
         <v>53</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>56</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>55</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J52" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>3</v>
-      </c>
-      <c r="B54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J54" t="s">
-        <v>197</v>
+      <c r="J53" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
         <v>36</v>
@@ -3526,30 +3538,30 @@
         <v>57</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="J56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3557,95 +3569,115 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="J57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J58" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>6</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>35</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>128</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>129</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J58" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="9" t="s">
+      <c r="J59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-    </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F25" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F29" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F43" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F57" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F50" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F51" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F52" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F54" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F55" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="J46" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F44" r:id="rId15" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
-    <hyperlink ref="F48" r:id="rId16" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
-    <hyperlink ref="F19" r:id="rId18" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
-    <hyperlink ref="J19" r:id="rId19" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
-    <hyperlink ref="J18" r:id="rId20" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
-    <hyperlink ref="F20" r:id="rId21" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
-    <hyperlink ref="F45" r:id="rId22" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
-    <hyperlink ref="J47" r:id="rId23" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
-    <hyperlink ref="F42" r:id="rId24" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
+    <hyperlink ref="F22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F25" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J29" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F44" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F58" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F51" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F52" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F53" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F55" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F56" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J47" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F45" r:id="rId15" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
+    <hyperlink ref="F49" r:id="rId16" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
+    <hyperlink ref="J19" r:id="rId20" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
+    <hyperlink ref="F21" r:id="rId21" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
+    <hyperlink ref="F46" r:id="rId22" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
+    <hyperlink ref="J48" r:id="rId23" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
+    <hyperlink ref="F43" r:id="rId24" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
     <hyperlink ref="J6" r:id="rId25" xr:uid="{9E0ED9E0-C3A3-4348-BB6F-5C429B9E61E7}"/>
     <hyperlink ref="J14" r:id="rId26" xr:uid="{AC848EF4-7FAB-4E48-AF09-F798B5BC950A}"/>
     <hyperlink ref="J8" r:id="rId27" xr:uid="{238CA172-A99C-46CD-9FBB-BE7CBE8D9023}"/>
@@ -3659,25 +3691,25 @@
     <hyperlink ref="F16" r:id="rId35" xr:uid="{5A1179F6-3A84-498D-87AF-DBF1D5EAF071}"/>
     <hyperlink ref="F9" r:id="rId36" xr:uid="{F2E3BA95-EDCE-4952-9E03-A8804711C4CB}"/>
     <hyperlink ref="F11" r:id="rId37" xr:uid="{4C536C75-1E7B-4E8E-AC70-3B143F26311E}"/>
-    <hyperlink ref="F17" r:id="rId38" xr:uid="{9DE94678-EFDC-4596-B004-CE73B42552E7}"/>
-    <hyperlink ref="J17" r:id="rId39" xr:uid="{22025D74-97DB-4D2B-BB71-13FAD64FC821}"/>
-    <hyperlink ref="F26" r:id="rId40" xr:uid="{0DF77104-940B-4656-902E-D3B4A729F975}"/>
-    <hyperlink ref="F30" r:id="rId41" xr:uid="{0234E1EC-3124-4C89-975E-D13FE095B07F}"/>
-    <hyperlink ref="F31" r:id="rId42" xr:uid="{DB5928A3-0C2C-41C8-94E2-173BFEB2B0BB}"/>
-    <hyperlink ref="F32" r:id="rId43" xr:uid="{24D2838B-698C-49F3-A89F-82FDF5909F9B}"/>
-    <hyperlink ref="F33" r:id="rId44" xr:uid="{5354C7EC-6A56-490A-97A1-06170A361210}"/>
-    <hyperlink ref="J27" r:id="rId45" xr:uid="{DA65564B-FC06-44AA-BE9E-CDEC85344EA4}"/>
-    <hyperlink ref="F36" r:id="rId46" xr:uid="{9B529563-7FF1-4CBB-B28F-CF26D80CBBD0}"/>
-    <hyperlink ref="F37" r:id="rId47" xr:uid="{19B2C35A-2AC5-48E0-ADAA-8A862A2BE8D1}"/>
-    <hyperlink ref="F39" r:id="rId48" xr:uid="{95AFB553-4A2D-4412-8ADD-9C777E0114C2}"/>
-    <hyperlink ref="F40" r:id="rId49" xr:uid="{B4A17999-A824-419D-96B6-45991272181C}"/>
-    <hyperlink ref="F38" r:id="rId50" xr:uid="{748FCFF4-A3F0-42DC-A53F-B6C8D0F870A5}"/>
-    <hyperlink ref="F35" r:id="rId51" xr:uid="{8CE5E525-65D3-417D-A66F-FDAA297CA9FB}"/>
-    <hyperlink ref="F34" r:id="rId52" xr:uid="{DF66115C-265B-4566-AA35-F0AD032F438C}"/>
-    <hyperlink ref="F41" r:id="rId53" xr:uid="{932A7A9F-0EC3-41B4-8980-42A6D5FC0033}"/>
-    <hyperlink ref="F58" r:id="rId54" xr:uid="{7A52BB5F-2156-4696-A05E-A65CF92F76E9}"/>
-    <hyperlink ref="F56" r:id="rId55" xr:uid="{2CBD1E2B-EA04-41D5-947D-738E19704CE1}"/>
-    <hyperlink ref="F22" r:id="rId56" xr:uid="{D7D22B2B-3A31-4EBC-A56A-9A899E1E05E5}"/>
+    <hyperlink ref="F18" r:id="rId38" xr:uid="{9DE94678-EFDC-4596-B004-CE73B42552E7}"/>
+    <hyperlink ref="J18" r:id="rId39" xr:uid="{22025D74-97DB-4D2B-BB71-13FAD64FC821}"/>
+    <hyperlink ref="F27" r:id="rId40" xr:uid="{0DF77104-940B-4656-902E-D3B4A729F975}"/>
+    <hyperlink ref="F31" r:id="rId41" xr:uid="{0234E1EC-3124-4C89-975E-D13FE095B07F}"/>
+    <hyperlink ref="F32" r:id="rId42" xr:uid="{DB5928A3-0C2C-41C8-94E2-173BFEB2B0BB}"/>
+    <hyperlink ref="F33" r:id="rId43" xr:uid="{24D2838B-698C-49F3-A89F-82FDF5909F9B}"/>
+    <hyperlink ref="F34" r:id="rId44" xr:uid="{5354C7EC-6A56-490A-97A1-06170A361210}"/>
+    <hyperlink ref="J28" r:id="rId45" xr:uid="{DA65564B-FC06-44AA-BE9E-CDEC85344EA4}"/>
+    <hyperlink ref="F37" r:id="rId46" xr:uid="{9B529563-7FF1-4CBB-B28F-CF26D80CBBD0}"/>
+    <hyperlink ref="F38" r:id="rId47" xr:uid="{19B2C35A-2AC5-48E0-ADAA-8A862A2BE8D1}"/>
+    <hyperlink ref="F40" r:id="rId48" xr:uid="{95AFB553-4A2D-4412-8ADD-9C777E0114C2}"/>
+    <hyperlink ref="F41" r:id="rId49" xr:uid="{B4A17999-A824-419D-96B6-45991272181C}"/>
+    <hyperlink ref="F39" r:id="rId50" xr:uid="{748FCFF4-A3F0-42DC-A53F-B6C8D0F870A5}"/>
+    <hyperlink ref="F36" r:id="rId51" xr:uid="{8CE5E525-65D3-417D-A66F-FDAA297CA9FB}"/>
+    <hyperlink ref="F35" r:id="rId52" xr:uid="{DF66115C-265B-4566-AA35-F0AD032F438C}"/>
+    <hyperlink ref="F42" r:id="rId53" xr:uid="{932A7A9F-0EC3-41B4-8980-42A6D5FC0033}"/>
+    <hyperlink ref="F59" r:id="rId54" xr:uid="{7A52BB5F-2156-4696-A05E-A65CF92F76E9}"/>
+    <hyperlink ref="F57" r:id="rId55" xr:uid="{2CBD1E2B-EA04-41D5-947D-738E19704CE1}"/>
+    <hyperlink ref="F23" r:id="rId56" xr:uid="{D7D22B2B-3A31-4EBC-A56A-9A899E1E05E5}"/>
     <hyperlink ref="F15" r:id="rId57" xr:uid="{67316A66-E885-4019-9B97-023E307D9CB3}"/>
     <hyperlink ref="F3" r:id="rId58" xr:uid="{B02C8DF0-BB09-4FA6-B67E-C7A7B9EEB465}"/>
     <hyperlink ref="F4" r:id="rId59" xr:uid="{BB0BB101-C150-49C2-8F2D-51BB0D499267}"/>
@@ -3688,16 +3720,18 @@
     <hyperlink ref="F12" r:id="rId64" xr:uid="{E6F9E951-725F-496F-8A3A-9F5DA1D9E614}"/>
     <hyperlink ref="F13" r:id="rId65" xr:uid="{DB9D0360-FD3F-451A-A90D-5E3B558DF116}"/>
     <hyperlink ref="F14" r:id="rId66" xr:uid="{2E579FF5-E003-4DED-AF14-BFC5B0D4309E}"/>
-    <hyperlink ref="F28" r:id="rId67" xr:uid="{62F7C14B-AFF7-4188-B463-597C440C8DE9}"/>
-    <hyperlink ref="F27" r:id="rId68" xr:uid="{A0AE6722-7DAF-47AF-9D23-B4599823780B}"/>
-    <hyperlink ref="F47" r:id="rId69" xr:uid="{3162AEA0-F325-498D-B7F8-4E76C8A146C1}"/>
-    <hyperlink ref="F46" r:id="rId70" xr:uid="{37C42E84-80D8-4CD9-A64C-BAD19903C9A5}"/>
+    <hyperlink ref="F29" r:id="rId67" xr:uid="{62F7C14B-AFF7-4188-B463-597C440C8DE9}"/>
+    <hyperlink ref="F28" r:id="rId68" xr:uid="{A0AE6722-7DAF-47AF-9D23-B4599823780B}"/>
+    <hyperlink ref="F48" r:id="rId69" xr:uid="{3162AEA0-F325-498D-B7F8-4E76C8A146C1}"/>
+    <hyperlink ref="F47" r:id="rId70" xr:uid="{37C42E84-80D8-4CD9-A64C-BAD19903C9A5}"/>
     <hyperlink ref="J10" r:id="rId71" xr:uid="{D8AF967F-D44E-42C9-8F2B-D5EB9F8AAAD4}"/>
     <hyperlink ref="J15" r:id="rId72" xr:uid="{35FE4693-DDA3-4377-A2A9-B5A4BE55BB87}"/>
     <hyperlink ref="J16" r:id="rId73" xr:uid="{D6346564-BC0F-4791-86F5-BE2F1D426945}"/>
+    <hyperlink ref="F17" r:id="rId74" xr:uid="{BE8BCBD6-1941-4587-8CEA-0C29F0C509F9}"/>
+    <hyperlink ref="J17" r:id="rId75" xr:uid="{3C36A0C5-6472-4EF1-9153-9339A6F47B44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
-  <drawing r:id="rId75"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
+  <drawing r:id="rId77"/>
 </worksheet>
 </file>
</xml_diff>